<commit_message>
to see if this is working
is it working
</commit_message>
<xml_diff>
--- a/binaural data.xlsx
+++ b/binaural data.xlsx
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -228,6 +228,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,7 +529,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -634,6 +637,9 @@
       </c>
       <c r="Q2" s="2">
         <v>4</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="39.75" thickBot="1">

</xml_diff>